<commit_message>
mejora en registro y dashboard
</commit_message>
<xml_diff>
--- a/public/files/Inscripciones.xlsx
+++ b/public/files/Inscripciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\SENA 2019\SENASOFT\senasoft\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CE365E-CB61-4C2E-B1DF-3F94B317BBBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2063A617-899F-4214-8C56-B350E571ED9A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{651F0DA9-E344-416E-B1D5-ED022C759C81}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="1186">
   <si>
     <t>Tipo Documento</t>
   </si>
@@ -3730,11 +3730,32 @@
       <t>*</t>
     </r>
   </si>
+  <si>
+    <t>juan</t>
+  </si>
+  <si>
+    <t>david</t>
+  </si>
+  <si>
+    <t>sdfds</t>
+  </si>
+  <si>
+    <t>kkl</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>kj</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3818,7 +3839,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3836,6 +3857,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4223,8 +4247,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4248,9 +4272,9 @@
     <col min="19" max="19" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:19" s="7" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:19" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:19" s="8" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:19" s="9" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:19" s="1" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>1168</v>
@@ -4312,29 +4336,47 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="6">
+      <c r="C5" s="2">
+        <v>1152694464</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F5" s="7">
         <v>34735</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>1182</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>1183</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>1184</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>1185</v>
+      </c>
       <c r="K5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="2">
+        <v>54654</v>
+      </c>
       <c r="M5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2">
+        <v>54</v>
+      </c>
       <c r="O5" s="2" t="s">
         <v>25</v>
       </c>

</xml_diff>